<commit_message>
affichage des playlists et lecture des morceaux d'une playlist
</commit_message>
<xml_diff>
--- a/documentation/audiofileplayer_planning.xlsx
+++ b/documentation/audiofileplayer_planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="20">
   <si>
     <t>AudioFile Player</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Analyse globale</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -25293,7 +25296,7 @@
   <dimension ref="A1:Y998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -25626,7 +25629,9 @@
       <c r="B12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
       <c r="D12" s="14"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -25637,8 +25642,12 @@
       <c r="K12" s="16"/>
       <c r="L12" s="29"/>
       <c r="M12" s="15"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="15"/>
+      <c r="N12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="41"/>
       <c r="R12" s="8"/>
@@ -25833,7 +25842,7 @@
       <c r="B17" s="3"/>
       <c r="C17" s="20">
         <f>SUM(C7:C16)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>

</xml_diff>

<commit_message>
màj de la documentation_technique et manuel_utilisateur
</commit_message>
<xml_diff>
--- a/documentation/audiofileplayer_planning.xlsx
+++ b/documentation/audiofileplayer_planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
   <si>
     <t>AudioFile Player</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Planification réel</t>
   </si>
 </sst>
 </file>
@@ -25296,7 +25299,7 @@
   <dimension ref="A1:Y998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -25381,7 +25384,7 @@
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="A4" s="49" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="4"/>
@@ -25664,7 +25667,9 @@
       <c r="B13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="23">
+        <v>0.5</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -25677,7 +25682,9 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="P13" s="29" t="s">
+        <v>5</v>
+      </c>
       <c r="Q13" s="42"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
@@ -25693,7 +25700,9 @@
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="24">
+        <v>0.5</v>
+      </c>
       <c r="D14" s="14"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -25707,7 +25716,9 @@
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
       <c r="P14" s="29"/>
-      <c r="Q14" s="42"/>
+      <c r="Q14" s="42" t="s">
+        <v>5</v>
+      </c>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
@@ -25842,7 +25853,7 @@
       <c r="B17" s="3"/>
       <c r="C17" s="20">
         <f>SUM(C7:C16)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>

</xml_diff>